<commit_message>
finding invalid offers from Excel and savinf to output.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/InvalidOffers.xlsx
+++ b/src/main/resources/InvalidOffers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanku\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\yuvi\java\STS\OfferIssue\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B70042-8B36-44E7-9949-67026D338D5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA41ADF-EF16-4A3C-8652-9D4D9ED7878E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>uiuiuihgvgvfgvc354648585</t>
   </si>
@@ -39,15 +39,6 @@
     <t>9876543ERTY</t>
   </si>
   <si>
-    <t>OLOLOL$565656</t>
-  </si>
-  <si>
-    <t>UIUIGCBHV$</t>
-  </si>
-  <si>
-    <t>909090O^&gt;LOLOLO</t>
-  </si>
-  <si>
     <t>78765453OLIKUJ</t>
   </si>
   <si>
@@ -61,9 +52,6 @@
   </si>
   <si>
     <t>IOIOPO987</t>
-  </si>
-  <si>
-    <t>UIUIUIOI89</t>
   </si>
   <si>
     <t>9876543*&amp;*&amp;ERTY</t>
@@ -384,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -401,7 +389,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1">
         <v>3</v>
@@ -418,56 +406,36 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
invalid number of offres also added to output.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/InvalidOffers.xlsx
+++ b/src/main/resources/InvalidOffers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\yuvi\java\STS\OfferIssue\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA41ADF-EF16-4A3C-8652-9D4D9ED7878E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1657FBC0-430D-4A41-87EA-831FDEC755C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>uiuiuihgvgvfgvc354648585</t>
   </si>
@@ -55,6 +55,30 @@
   </si>
   <si>
     <t>9876543*&amp;*&amp;ERTY</t>
+  </si>
+  <si>
+    <t>ABCHJUH</t>
+  </si>
+  <si>
+    <t>909ikokujyhtgt*</t>
+  </si>
+  <si>
+    <t>JKJKUHY/////\\\\\%^%gyvb</t>
+  </si>
+  <si>
+    <t>iojkjkjhjhjhjjhj</t>
+  </si>
+  <si>
+    <t>ioiojkhjghfgfgghbn</t>
+  </si>
+  <si>
+    <t>jkjkhjhh)))))</t>
+  </si>
+  <si>
+    <t>(((hjnmnmnmm####</t>
+  </si>
+  <si>
+    <t>hjhj.uiuiuisdksd</t>
   </si>
 </sst>
 </file>
@@ -372,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -385,9 +409,10 @@
     <col min="3" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -404,7 +429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -424,7 +449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -436,6 +461,35 @@
       </c>
       <c r="D3" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>